<commit_message>
crea carpeta con la ficha para guardar y seguir generando
</commit_message>
<xml_diff>
--- a/BACKEND/plantilla.xlsx
+++ b/BACKEND/plantilla.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,7 @@
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="13" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -470,6 +471,11 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>AÑO</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>FICHA</t>
         </is>
       </c>
     </row>

</xml_diff>